<commit_message>
Update on several resources (no good commit) Added translations for Anamnese
</commit_message>
<xml_diff>
--- a/olafia/2 Anamnese/Engelsk oversettelse Selvregistreringsskjemaet Anne og Patricia.xlsx
+++ b/olafia/2 Anamnese/Engelsk oversettelse Selvregistreringsskjemaet Anne og Patricia.xlsx
@@ -1359,9 +1359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1411,7 +1409,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1540,7 +1538,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1563,7 +1561,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1626,7 +1624,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2119,7 +2117,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2136,7 +2134,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2958,7 +2956,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2981,7 +2979,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>

</xml_diff>